<commit_message>
Redo the calcs in the spreadsheet, add test image files.
</commit_message>
<xml_diff>
--- a/Neopixel Calculations.xlsx
+++ b/Neopixel Calculations.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdomoney/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdomoney/Projects/hackathon11fastled/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pre-resize" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>X</t>
   </si>
@@ -69,6 +70,18 @@
   </si>
   <si>
     <t>Current (A)</t>
+  </si>
+  <si>
+    <t>LED spacing</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>LED count</t>
   </si>
 </sst>
 </file>
@@ -112,9 +125,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,4 +633,140 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3">
+        <f>B1/B2</f>
+        <v>1.3216957605985038</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f>B1*B2</f>
+        <v>212530</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>80385</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>36492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <f>(B6+B7)/B4</f>
+        <v>0.54993177433774054</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3">
+        <v>33.333300000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3">
+        <f>B10*B10</f>
+        <v>1111.1088888900001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="4">
+        <v>985</v>
+      </c>
+      <c r="C14" s="4">
+        <f>B14*B3</f>
+        <v>1301.8703241895262</v>
+      </c>
+      <c r="D14" s="4">
+        <f>ROUNDDOWN(B14/B10,0)</f>
+        <v>29</v>
+      </c>
+      <c r="E14" s="4">
+        <f>ROUNDDOWN(C14/B10,0)</f>
+        <v>39</v>
+      </c>
+      <c r="F14" s="4">
+        <f>D14*E14*B8</f>
+        <v>621.97283677598455</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>